<commit_message>
In progress edits to add two new hydrogen production pathways
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HPEC/Hydrogen Production Eqpt Costs.xlsx
+++ b/InputData/hydgn/HPEC/Hydrogen Production Eqpt Costs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\hydgn\HPEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\hydgn\HPEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144CF766-F142-4FDB-B3C8-5736800C38EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11970"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,17 +24,28 @@
     <definedName name="hours_per_year">'Conversion Factors'!$A$1</definedName>
     <definedName name="usd_year_conv">'Conversion Factors'!$A$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>HPEC Hydrogen Production Equipment CapEx</t>
   </si>
@@ -273,11 +285,17 @@
   <si>
     <t>OpEx Cost ($/BTU)</t>
   </si>
+  <si>
+    <t>electrolysis with guaranteed clean electricity</t>
+  </si>
+  <si>
+    <t>natural gas reforming with CCS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -377,16 +395,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -667,29 +678,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.86328125" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -697,230 +708,230 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" s="7">
         <v>2014</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B39" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B39" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -928,20 +939,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.3984375" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" customWidth="1"/>
-    <col min="5" max="5" width="10.1328125" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="1" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -961,7 +972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -981,7 +992,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -998,7 +1009,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -1015,7 +1026,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
@@ -1033,7 +1044,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1053,7 +1064,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1070,7 +1081,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1087,7 +1098,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -1105,7 +1116,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1125,7 +1136,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1142,7 +1153,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1170,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -1177,8 +1188,8 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1198,14 +1209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>24*365</f>
         <v>8760</v>
@@ -1214,7 +1225,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3412.14</v>
       </c>
@@ -1222,7 +1233,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.91400000000000003</v>
       </c>
@@ -1236,20 +1247,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
@@ -1292,7 +1305,7 @@
       <c r="N1" s="9">
         <v>2029</v>
       </c>
-      <c r="O1" s="13">
+      <c r="O1" s="12">
         <v>2030</v>
       </c>
       <c r="P1" s="10">
@@ -1356,708 +1369,990 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,B$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7520591062805481E-5</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,C$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7050153608740382E-5</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,D$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.6579716154675392E-5</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,E$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.6109278700610286E-5</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,F$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.5638841246545299E-5</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,G$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.5168403792480193E-5</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,H$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.469796633841509E-5</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,I$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.4227528884350103E-5</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,J$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.3757091430284997E-5</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,K$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.328665397622001E-5</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,L$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.2816216522154904E-5</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,M$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.2345779068089914E-5</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,N$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.1875341614024811E-5</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="11">
         <f>TREND('IEA Data'!$D2:$E2,'IEA Data'!$D$15:$E$15,O$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.1404904159959821E-5</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="13">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,P$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.1022673728531968E-5</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,Q$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.0640443297104115E-5</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,R$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.0258212865676262E-5</v>
       </c>
-      <c r="S2" s="12">
+      <c r="S2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,S$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.9875982434248403E-5</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,T$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.949375200282055E-5</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,U$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.9111521571392698E-5</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,V$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.8729291139964845E-5</v>
       </c>
-      <c r="W2" s="12">
+      <c r="W2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,W$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.8347060708536989E-5</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,X$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.7964830277109136E-5</v>
       </c>
-      <c r="Y2" s="12">
+      <c r="Y2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,Y$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.7582599845681283E-5</v>
       </c>
-      <c r="Z2" s="12">
+      <c r="Z2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,Z$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.7200369414253427E-5</v>
       </c>
-      <c r="AA2" s="12">
+      <c r="AA2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AA$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.6818138982825571E-5</v>
       </c>
-      <c r="AB2" s="12">
+      <c r="AB2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AB$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.6435908551397718E-5</v>
       </c>
-      <c r="AC2" s="12">
+      <c r="AC2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AC$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.6053678119969865E-5</v>
       </c>
-      <c r="AD2" s="12">
+      <c r="AD2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AD$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.5671447688542013E-5</v>
       </c>
-      <c r="AE2" s="12">
+      <c r="AE2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AE$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.5289217257114157E-5</v>
       </c>
-      <c r="AF2" s="12">
+      <c r="AF2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AF$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.4906986825686302E-5</v>
       </c>
-      <c r="AG2" s="12">
+      <c r="AG2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AG$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.4524756394258449E-5</v>
       </c>
-      <c r="AH2" s="12">
+      <c r="AH2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AH$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.4142525962830597E-5</v>
       </c>
-      <c r="AI2" s="12">
+      <c r="AI2" s="11">
         <f>TREND('IEA Data'!$E2:$F2,'IEA Data'!$E$15:$F$15,AI$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>1.3760295531402741E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,B$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,C$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,D$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,E$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,F$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,G$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,H$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,I$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,J$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,K$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,L$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,M$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,N$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="11">
         <f>TREND('IEA Data'!$D6:$E6,'IEA Data'!$D$15:$E$15,O$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="13">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,P$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,Q$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,R$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="S3" s="12">
+      <c r="S3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,S$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,T$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,U$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="V3" s="12">
+      <c r="V3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,V$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,W$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,X$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Y3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,Y$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="Z3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,Z$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AA$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AB3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AB$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AC3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AC$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AD3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AD$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AE$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AF3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AF$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AG3" s="12">
+      <c r="AG3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AG$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AH3" s="12">
+      <c r="AH3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AH$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
-      <c r="AI3" s="12">
+      <c r="AI3" s="11">
         <f>TREND('IEA Data'!$E6:$F6,'IEA Data'!$E$15:$F$15,AI$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>2.7826375407947768E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,B$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,C$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,D$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,E$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,F$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,G$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,H$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,I$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,J$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,K$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,L$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,M$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,N$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="11">
         <f>TREND('IEA Data'!$D10:$E10,'IEA Data'!$D$15:$E$15,O$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="13">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,P$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,Q$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,R$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="S4" s="12">
+      <c r="S4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,S$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,T$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="U4" s="12">
+      <c r="U4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,U$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="V4" s="12">
+      <c r="V4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,V$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="W4" s="12">
+      <c r="W4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,W$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="X4" s="12">
+      <c r="X4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,X$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="Y4" s="12">
+      <c r="Y4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,Y$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="Z4" s="12">
+      <c r="Z4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,Z$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AA4" s="12">
+      <c r="AA4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AA$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AB4" s="12">
+      <c r="AB4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AB$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AC4" s="12">
+      <c r="AC4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AC$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AD4" s="12">
+      <c r="AD4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AD$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AE4" s="12">
+      <c r="AE4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AE$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AF4" s="12">
+      <c r="AF4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AF$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AG4" s="12">
+      <c r="AG4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AG$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AH4" s="12">
+      <c r="AH4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AH$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AI4" s="12">
+      <c r="AI4" s="11">
         <f>TREND('IEA Data'!$E10:$F10,'IEA Data'!$E$15:$F$15,AI$1)/hours_per_year/btu_per_kwh*usd_year_conv</f>
         <v>8.1644420152989595E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <f t="shared" ref="C5:P5" si="0">C4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="D5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="E5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="F5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="G5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="H5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="I5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="J5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="K5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="L5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="M5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="N5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="O5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="P5" s="12">
-        <f t="shared" si="0"/>
-        <v>8.1644420152989595E-5</v>
-      </c>
-      <c r="Q5" s="12">
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1644420152989595E-5</v>
+      </c>
+      <c r="Q5" s="11">
         <f t="shared" ref="Q5" si="1">Q4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="R5" s="12">
+      <c r="R5" s="11">
         <f t="shared" ref="R5" si="2">R4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="S5" s="12">
+      <c r="S5" s="11">
         <f t="shared" ref="S5" si="3">S4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="11">
         <f t="shared" ref="T5" si="4">T4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="11">
         <f t="shared" ref="U5" si="5">U4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="V5" s="12">
+      <c r="V5" s="11">
         <f t="shared" ref="V5" si="6">V4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="W5" s="12">
+      <c r="W5" s="11">
         <f t="shared" ref="W5" si="7">W4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="X5" s="12">
+      <c r="X5" s="11">
         <f t="shared" ref="X5" si="8">X4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="Y5" s="12">
+      <c r="Y5" s="11">
         <f t="shared" ref="Y5" si="9">Y4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="Z5" s="12">
+      <c r="Z5" s="11">
         <f t="shared" ref="Z5" si="10">Z4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="11">
         <f t="shared" ref="AA5" si="11">AA4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AB5" s="12">
+      <c r="AB5" s="11">
         <f t="shared" ref="AB5" si="12">AB4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AC5" s="12">
+      <c r="AC5" s="11">
         <f t="shared" ref="AC5" si="13">AC4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AD5" s="12">
+      <c r="AD5" s="11">
         <f t="shared" ref="AD5" si="14">AD4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AE5" s="12">
+      <c r="AE5" s="11">
         <f t="shared" ref="AE5" si="15">AE4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AF5" s="12">
+      <c r="AF5" s="11">
         <f t="shared" ref="AF5" si="16">AF4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AG5" s="12">
+      <c r="AG5" s="11">
         <f t="shared" ref="AG5" si="17">AG4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AH5" s="12">
+      <c r="AH5" s="11">
         <f t="shared" ref="AH5" si="18">AH4</f>
         <v>8.1644420152989595E-5</v>
       </c>
-      <c r="AI5" s="12">
+      <c r="AI5" s="11">
         <f t="shared" ref="AI5" si="19">AI4</f>
         <v>8.1644420152989595E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="11">
-        <v>0</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <f t="shared" ref="C6:R6" si="20">$B6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="Q6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6">
         <f t="shared" ref="S6:AI6" si="21">$B6</f>
         <v>0</v>
       </c>
-      <c r="T6" s="11">
+      <c r="T6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U6" s="11">
+      <c r="U6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="W6" s="11">
+      <c r="W6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AA6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AD6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="11">
+      <c r="AE6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AF6" s="11">
+      <c r="AF6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="11">
+      <c r="AG6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AH6" s="11">
+      <c r="AH6">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AI6" s="11">
+      <c r="AI6">
         <f t="shared" si="21"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="11">
+        <f>B2</f>
+        <v>2.7520591062805481E-5</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" ref="C7:AI7" si="22">C2</f>
+        <v>2.7050153608740382E-5</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.6579716154675392E-5</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.6109278700610286E-5</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.5638841246545299E-5</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.5168403792480193E-5</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.469796633841509E-5</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.4227528884350103E-5</v>
+      </c>
+      <c r="J7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.3757091430284997E-5</v>
+      </c>
+      <c r="K7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.328665397622001E-5</v>
+      </c>
+      <c r="L7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.2816216522154904E-5</v>
+      </c>
+      <c r="M7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.2345779068089914E-5</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.1875341614024811E-5</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.1404904159959821E-5</v>
+      </c>
+      <c r="P7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.1022673728531968E-5</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.0640443297104115E-5</v>
+      </c>
+      <c r="R7" s="11">
+        <f t="shared" si="22"/>
+        <v>2.0258212865676262E-5</v>
+      </c>
+      <c r="S7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.9875982434248403E-5</v>
+      </c>
+      <c r="T7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.949375200282055E-5</v>
+      </c>
+      <c r="U7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.9111521571392698E-5</v>
+      </c>
+      <c r="V7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.8729291139964845E-5</v>
+      </c>
+      <c r="W7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.8347060708536989E-5</v>
+      </c>
+      <c r="X7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.7964830277109136E-5</v>
+      </c>
+      <c r="Y7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.7582599845681283E-5</v>
+      </c>
+      <c r="Z7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.7200369414253427E-5</v>
+      </c>
+      <c r="AA7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.6818138982825571E-5</v>
+      </c>
+      <c r="AB7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.6435908551397718E-5</v>
+      </c>
+      <c r="AC7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.6053678119969865E-5</v>
+      </c>
+      <c r="AD7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.5671447688542013E-5</v>
+      </c>
+      <c r="AE7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.5289217257114157E-5</v>
+      </c>
+      <c r="AF7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.4906986825686302E-5</v>
+      </c>
+      <c r="AG7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.4524756394258449E-5</v>
+      </c>
+      <c r="AH7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.4142525962830597E-5</v>
+      </c>
+      <c r="AI7" s="11">
+        <f t="shared" si="22"/>
+        <v>1.3760295531402741E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="11">
+        <f>B3</f>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" ref="C8:AI8" si="23">C3</f>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="L8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="M8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="O8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="P8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="R8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="S8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="T8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="U8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="V8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="W8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="X8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="Y8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="Z8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AA8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AB8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AC8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AD8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AE8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AF8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AG8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AH8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
+      </c>
+      <c r="AI8" s="11">
+        <f t="shared" si="23"/>
+        <v>2.7826375407947768E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2066,828 +2361,1112 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AI8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="15">
+      <c r="B1" s="9">
         <v>2017</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1">
         <v>2018</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="9">
         <v>2019</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1">
         <v>2020</v>
       </c>
-      <c r="F1" s="15">
+      <c r="F1" s="9">
         <v>2021</v>
       </c>
-      <c r="G1" s="16">
+      <c r="G1">
         <v>2022</v>
       </c>
-      <c r="H1" s="15">
+      <c r="H1" s="9">
         <v>2023</v>
       </c>
-      <c r="I1" s="16">
+      <c r="I1">
         <v>2024</v>
       </c>
-      <c r="J1" s="15">
+      <c r="J1" s="9">
         <v>2025</v>
       </c>
-      <c r="K1" s="16">
+      <c r="K1">
         <v>2026</v>
       </c>
-      <c r="L1" s="15">
+      <c r="L1" s="9">
         <v>2027</v>
       </c>
-      <c r="M1" s="16">
+      <c r="M1">
         <v>2028</v>
       </c>
-      <c r="N1" s="15">
+      <c r="N1" s="9">
         <v>2029</v>
       </c>
-      <c r="O1" s="16">
+      <c r="O1">
         <v>2030</v>
       </c>
-      <c r="P1" s="15">
+      <c r="P1" s="9">
         <v>2031</v>
       </c>
-      <c r="Q1" s="16">
+      <c r="Q1">
         <v>2032</v>
       </c>
-      <c r="R1" s="15">
+      <c r="R1" s="9">
         <v>2033</v>
       </c>
-      <c r="S1" s="16">
+      <c r="S1">
         <v>2034</v>
       </c>
-      <c r="T1" s="15">
+      <c r="T1" s="9">
         <v>2035</v>
       </c>
-      <c r="U1" s="16">
+      <c r="U1">
         <v>2036</v>
       </c>
-      <c r="V1" s="15">
+      <c r="V1" s="9">
         <v>2037</v>
       </c>
-      <c r="W1" s="16">
+      <c r="W1">
         <v>2038</v>
       </c>
-      <c r="X1" s="15">
+      <c r="X1" s="9">
         <v>2039</v>
       </c>
-      <c r="Y1" s="16">
+      <c r="Y1">
         <v>2040</v>
       </c>
-      <c r="Z1" s="15">
+      <c r="Z1" s="9">
         <v>2041</v>
       </c>
-      <c r="AA1" s="16">
+      <c r="AA1">
         <v>2042</v>
       </c>
-      <c r="AB1" s="15">
+      <c r="AB1" s="9">
         <v>2043</v>
       </c>
-      <c r="AC1" s="16">
+      <c r="AC1">
         <v>2044</v>
       </c>
-      <c r="AD1" s="15">
+      <c r="AD1" s="9">
         <v>2045</v>
       </c>
-      <c r="AE1" s="16">
+      <c r="AE1">
         <v>2046</v>
       </c>
-      <c r="AF1" s="15">
+      <c r="AF1" s="9">
         <v>2047</v>
       </c>
-      <c r="AG1" s="16">
+      <c r="AG1">
         <v>2048</v>
       </c>
-      <c r="AH1" s="15">
+      <c r="AH1" s="9">
         <v>2049</v>
       </c>
-      <c r="AI1" s="16">
+      <c r="AI1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="11">
         <f>HPEC!B2*'IEA Data'!$D$4</f>
         <v>4.1280886594208218E-7</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="11">
         <f>HPEC!C2*'IEA Data'!$D$4</f>
         <v>4.057523041311057E-7</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="11">
         <f>HPEC!D2*'IEA Data'!$D$4</f>
         <v>3.9869574232013086E-7</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="11">
         <f>HPEC!E2*'IEA Data'!$D$4</f>
         <v>3.9163918050915428E-7</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="11">
         <f>HPEC!F2*'IEA Data'!$D$4</f>
         <v>3.8458261869817944E-7</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="11">
         <f>HPEC!G2*'IEA Data'!$D$4</f>
         <v>3.7752605688720286E-7</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="11">
         <f>HPEC!H2*'IEA Data'!$D$4</f>
         <v>3.7046949507622632E-7</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="11">
         <f>HPEC!I2*'IEA Data'!$D$4</f>
         <v>3.6341293326525154E-7</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="11">
         <f>HPEC!J2*'IEA Data'!$D$4</f>
         <v>3.5635637145427495E-7</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="11">
         <f>HPEC!K2*'IEA Data'!$D$4</f>
         <v>3.4929980964330012E-7</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="11">
         <f>HPEC!L2*'IEA Data'!$D$4</f>
         <v>3.4224324783232353E-7</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="11">
         <f>HPEC!M2*'IEA Data'!$D$4</f>
         <v>3.3518668602134869E-7</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="11">
         <f>HPEC!N2*'IEA Data'!$D$4</f>
         <v>3.2813012421037216E-7</v>
       </c>
-      <c r="O2" s="17">
+      <c r="O2" s="11">
         <f>HPEC!O2*'IEA Data'!$D$4</f>
         <v>3.2107356239939732E-7</v>
       </c>
-      <c r="P2" s="17">
+      <c r="P2" s="11">
         <f>HPEC!P2*'IEA Data'!$D$4</f>
         <v>3.1534010592797952E-7</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="11">
         <f>HPEC!Q2*'IEA Data'!$D$4</f>
         <v>3.0960664945656172E-7</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="11">
         <f>HPEC!R2*'IEA Data'!$D$4</f>
         <v>3.0387319298514391E-7</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="11">
         <f>HPEC!S2*'IEA Data'!$D$4</f>
         <v>2.9813973651372606E-7</v>
       </c>
-      <c r="T2" s="17">
+      <c r="T2" s="11">
         <f>HPEC!T2*'IEA Data'!$D$4</f>
         <v>2.9240628004230825E-7</v>
       </c>
-      <c r="U2" s="17">
+      <c r="U2" s="11">
         <f>HPEC!U2*'IEA Data'!$D$4</f>
         <v>2.8667282357089045E-7</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="11">
         <f>HPEC!V2*'IEA Data'!$D$4</f>
         <v>2.8093936709947264E-7</v>
       </c>
-      <c r="W2" s="17">
+      <c r="W2" s="11">
         <f>HPEC!W2*'IEA Data'!$D$4</f>
         <v>2.7520591062805484E-7</v>
       </c>
-      <c r="X2" s="17">
+      <c r="X2" s="11">
         <f>HPEC!X2*'IEA Data'!$D$4</f>
         <v>2.6947245415663704E-7</v>
       </c>
-      <c r="Y2" s="17">
+      <c r="Y2" s="11">
         <f>HPEC!Y2*'IEA Data'!$D$4</f>
         <v>2.6373899768521923E-7</v>
       </c>
-      <c r="Z2" s="17">
+      <c r="Z2" s="11">
         <f>HPEC!Z2*'IEA Data'!$D$4</f>
         <v>2.5800554121380138E-7</v>
       </c>
-      <c r="AA2" s="17">
+      <c r="AA2" s="11">
         <f>HPEC!AA2*'IEA Data'!$D$4</f>
         <v>2.5227208474238357E-7</v>
       </c>
-      <c r="AB2" s="17">
+      <c r="AB2" s="11">
         <f>HPEC!AB2*'IEA Data'!$D$4</f>
         <v>2.4653862827096577E-7</v>
       </c>
-      <c r="AC2" s="17">
+      <c r="AC2" s="11">
         <f>HPEC!AC2*'IEA Data'!$D$4</f>
         <v>2.4080517179954797E-7</v>
       </c>
-      <c r="AD2" s="17">
+      <c r="AD2" s="11">
         <f>HPEC!AD2*'IEA Data'!$D$4</f>
         <v>2.3507171532813019E-7</v>
       </c>
-      <c r="AE2" s="17">
+      <c r="AE2" s="11">
         <f>HPEC!AE2*'IEA Data'!$D$4</f>
         <v>2.2933825885671233E-7</v>
       </c>
-      <c r="AF2" s="17">
+      <c r="AF2" s="11">
         <f>HPEC!AF2*'IEA Data'!$D$4</f>
         <v>2.2360480238529453E-7</v>
       </c>
-      <c r="AG2" s="17">
+      <c r="AG2" s="11">
         <f>HPEC!AG2*'IEA Data'!$D$4</f>
         <v>2.1787134591387672E-7</v>
       </c>
-      <c r="AH2" s="12">
+      <c r="AH2" s="11">
         <f>HPEC!AH2*'IEA Data'!$D$4</f>
         <v>2.1213788944245895E-7</v>
       </c>
-      <c r="AI2" s="12">
+      <c r="AI2" s="11">
         <f>HPEC!AI2*'IEA Data'!$D$4</f>
         <v>2.0640443297104109E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <f>HPEC!B3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="11">
         <f>HPEC!C3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="11">
         <f>HPEC!D3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="11">
         <f>HPEC!E3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="11">
         <f>HPEC!F3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="11">
         <f>HPEC!G3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="11">
         <f>HPEC!H3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="11">
         <f>HPEC!I3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="11">
         <f>HPEC!J3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="11">
         <f>HPEC!K3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="11">
         <f>HPEC!L3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="11">
         <f>HPEC!M3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="11">
         <f>HPEC!N3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="11">
         <f>HPEC!O3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="11">
         <f>HPEC!P3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="Q3" s="11">
         <f>HPEC!Q3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="R3" s="17">
+      <c r="R3" s="11">
         <f>HPEC!R3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="S3" s="17">
+      <c r="S3" s="11">
         <f>HPEC!S3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="11">
         <f>HPEC!T3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="11">
         <f>HPEC!U3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="11">
         <f>HPEC!V3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="W3" s="17">
+      <c r="W3" s="11">
         <f>HPEC!W3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="X3" s="17">
+      <c r="X3" s="11">
         <f>HPEC!X3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="Y3" s="17">
+      <c r="Y3" s="11">
         <f>HPEC!Y3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="Z3" s="17">
+      <c r="Z3" s="11">
         <f>HPEC!Z3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AA3" s="17">
+      <c r="AA3" s="11">
         <f>HPEC!AA3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AB3" s="17">
+      <c r="AB3" s="11">
         <f>HPEC!AB3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AC3" s="17">
+      <c r="AC3" s="11">
         <f>HPEC!AC3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AD3" s="17">
+      <c r="AD3" s="11">
         <f>HPEC!AD3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AE3" s="17">
+      <c r="AE3" s="11">
         <f>HPEC!AE3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AF3" s="17">
+      <c r="AF3" s="11">
         <f>HPEC!AF3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AG3" s="17">
+      <c r="AG3" s="11">
         <f>HPEC!AG3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AH3" s="17">
+      <c r="AH3" s="11">
         <f>HPEC!AH3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
-      <c r="AI3" s="17">
+      <c r="AI3" s="11">
         <f>HPEC!AI3*'IEA Data'!$D$8</f>
         <v>1.307839644173545E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="11">
         <f>HPEC!B4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="11">
         <f>HPEC!C4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="11">
         <f>HPEC!D4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="11">
         <f>HPEC!E4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="11">
         <f>HPEC!F4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="11">
         <f>HPEC!G4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="11">
         <f>HPEC!H4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="11">
         <f>HPEC!I4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="11">
         <f>HPEC!J4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="11">
         <f>HPEC!K4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="11">
         <f>HPEC!L4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="11">
         <f>HPEC!M4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="11">
         <f>HPEC!N4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="11">
         <f>HPEC!O4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="P4" s="17">
+      <c r="P4" s="11">
         <f>HPEC!P4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="Q4" s="11">
         <f>HPEC!Q4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="R4" s="17">
+      <c r="R4" s="11">
         <f>HPEC!R4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="S4" s="17">
+      <c r="S4" s="11">
         <f>HPEC!S4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="T4" s="17">
+      <c r="T4" s="11">
         <f>HPEC!T4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="U4" s="17">
+      <c r="U4" s="11">
         <f>HPEC!U4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="V4" s="17">
+      <c r="V4" s="11">
         <f>HPEC!V4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="W4" s="17">
+      <c r="W4" s="11">
         <f>HPEC!W4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="X4" s="17">
+      <c r="X4" s="11">
         <f>HPEC!X4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="Y4" s="17">
+      <c r="Y4" s="11">
         <f>HPEC!Y4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="Z4" s="17">
+      <c r="Z4" s="11">
         <f>HPEC!Z4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AA4" s="17">
+      <c r="AA4" s="11">
         <f>HPEC!AA4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AB4" s="17">
+      <c r="AB4" s="11">
         <f>HPEC!AB4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AC4" s="17">
+      <c r="AC4" s="11">
         <f>HPEC!AC4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AD4" s="17">
+      <c r="AD4" s="11">
         <f>HPEC!AD4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AE4" s="17">
+      <c r="AE4" s="11">
         <f>HPEC!AE4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AF4" s="17">
+      <c r="AF4" s="11">
         <f>HPEC!AF4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AG4" s="17">
+      <c r="AG4" s="11">
         <f>HPEC!AG4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AH4" s="12">
+      <c r="AH4" s="11">
         <f>HPEC!AH4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="AI4" s="12">
+      <c r="AI4" s="11">
         <f>HPEC!AI4*'IEA Data'!$D$12</f>
         <v>4.0822210076494796E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <f t="shared" ref="C5:AI5" si="0">C4</f>
         <v>4.0822210076494796E-6</v>
       </c>
-      <c r="D5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="E5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="F5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="G5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="H5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="I5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="J5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="K5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="L5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="M5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="N5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="O5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="P5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="Q5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="R5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="S5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="T5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="U5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="V5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="W5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="X5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="Y5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="Z5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AA5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AB5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AC5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AD5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AE5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AF5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AG5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AH5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-      <c r="AI5" s="12">
-        <f t="shared" si="0"/>
-        <v>4.0822210076494796E-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="R5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="S5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="T5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="U5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="V5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="W5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="X5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="Y5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="Z5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AA5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AB5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AC5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AD5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AE5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AF5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AG5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AH5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+      <c r="AI5" s="11">
+        <f t="shared" si="0"/>
+        <v>4.0822210076494796E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="11">
-        <v>0</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <f t="shared" ref="C6:AI6" si="1">$B6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="Q6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T6" s="11">
+      <c r="T6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U6" s="11">
+      <c r="U6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W6" s="11">
+      <c r="W6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AA6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AD6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="11">
+      <c r="AE6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF6" s="11">
+      <c r="AF6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="11">
+      <c r="AG6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH6" s="11">
+      <c r="AH6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AI6" s="11">
+      <c r="AI6">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="11">
+        <f>B2</f>
+        <v>4.1280886594208218E-7</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" ref="C7:AI7" si="2">C2</f>
+        <v>4.057523041311057E-7</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9869574232013086E-7</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9163918050915428E-7</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.8458261869817944E-7</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.7752605688720286E-7</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.7046949507622632E-7</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.6341293326525154E-7</v>
+      </c>
+      <c r="J7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.5635637145427495E-7</v>
+      </c>
+      <c r="K7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4929980964330012E-7</v>
+      </c>
+      <c r="L7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4224324783232353E-7</v>
+      </c>
+      <c r="M7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.3518668602134869E-7</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.2813012421037216E-7</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.2107356239939732E-7</v>
+      </c>
+      <c r="P7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.1534010592797952E-7</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.0960664945656172E-7</v>
+      </c>
+      <c r="R7" s="11">
+        <f t="shared" si="2"/>
+        <v>3.0387319298514391E-7</v>
+      </c>
+      <c r="S7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.9813973651372606E-7</v>
+      </c>
+      <c r="T7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.9240628004230825E-7</v>
+      </c>
+      <c r="U7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.8667282357089045E-7</v>
+      </c>
+      <c r="V7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.8093936709947264E-7</v>
+      </c>
+      <c r="W7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.7520591062805484E-7</v>
+      </c>
+      <c r="X7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.6947245415663704E-7</v>
+      </c>
+      <c r="Y7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.6373899768521923E-7</v>
+      </c>
+      <c r="Z7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.5800554121380138E-7</v>
+      </c>
+      <c r="AA7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.5227208474238357E-7</v>
+      </c>
+      <c r="AB7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4653862827096577E-7</v>
+      </c>
+      <c r="AC7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4080517179954797E-7</v>
+      </c>
+      <c r="AD7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.3507171532813019E-7</v>
+      </c>
+      <c r="AE7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.2933825885671233E-7</v>
+      </c>
+      <c r="AF7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.2360480238529453E-7</v>
+      </c>
+      <c r="AG7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.1787134591387672E-7</v>
+      </c>
+      <c r="AH7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.1213788944245895E-7</v>
+      </c>
+      <c r="AI7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.0640443297104109E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="11">
+        <f>B3</f>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" ref="C8:AI8" si="3">C3</f>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="L8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="M8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="O8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="P8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="R8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="S8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="T8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="U8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="V8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="W8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="X8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="Y8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="Z8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AA8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AB8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AC8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AD8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AE8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AF8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AG8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AH8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
+      </c>
+      <c r="AI8" s="11">
+        <f t="shared" si="3"/>
+        <v>1.307839644173545E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaces thermochemical water splitting hydrogen production pathway with partial oxidation of hydrocarbons
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HPEC/Hydrogen Production Eqpt Costs.xlsx
+++ b/InputData/hydgn/HPEC/Hydrogen Production Eqpt Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\hydgn\HPEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\HPEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144CF766-F142-4FDB-B3C8-5736800C38EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06FFE47-8401-4153-B365-3B8D108180A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30315" yWindow="315" windowWidth="21630" windowHeight="13245" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>biomass gasification</t>
   </si>
   <si>
-    <t>thermochemical water splitting</t>
-  </si>
-  <si>
     <t>hours per year</t>
   </si>
   <si>
@@ -188,27 +185,6 @@
     <t>Page 7, Table 3</t>
   </si>
   <si>
-    <t>Thermochemical Water Splitting</t>
-  </si>
-  <si>
-    <t>This technology can utilize heat from solar thermal (e.g. mirror</t>
-  </si>
-  <si>
-    <t>collectors, etc.) or from nuclear plants.  Capital costs would</t>
-  </si>
-  <si>
-    <t>vary greatly depending on the technology used.</t>
-  </si>
-  <si>
-    <t>This technology isn't used in the U.S. version of the model,</t>
-  </si>
-  <si>
-    <t>is available for EPS adaptations for other regions or future</t>
-  </si>
-  <si>
-    <t>U.S. region dataset updates.</t>
-  </si>
-  <si>
     <t>2018 USD/2012 USD</t>
   </si>
   <si>
@@ -222,9 +198,6 @@
   </si>
   <si>
     <t>HPEC Hydrogen Production Equipment OpEx</t>
-  </si>
-  <si>
-    <t>so no costs are included here, but the subscript element</t>
   </si>
   <si>
     <t>In other words, this variable should contain the CapEx</t>
@@ -290,6 +263,33 @@
   </si>
   <si>
     <t>natural gas reforming with CCS</t>
+  </si>
+  <si>
+    <t>hydrocarbon partial oxidation</t>
+  </si>
+  <si>
+    <t>Partial Oxidation of Hydrocarbons</t>
+  </si>
+  <si>
+    <t>According to ICF, POx reactors are essentially equivalent to autothermal</t>
+  </si>
+  <si>
+    <t>reformers (ATRs) but without a catalyst bed. For lack of economic data,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we assume that the costs mirror those of ATRs, which, per ICF, </t>
+  </si>
+  <si>
+    <t>Robertson, Penshorn, and McCurdy</t>
+  </si>
+  <si>
+    <t>Comparing the costs of industrial hydrogen technologies</t>
+  </si>
+  <si>
+    <t>https://www.icf.com/insights/energy/comparing-costs-of-industrial-hydrogen-technologies</t>
+  </si>
+  <si>
+    <t>have ~15% lower capital costs and ~5% lower production costs than SMRs.</t>
   </si>
 </sst>
 </file>
@@ -679,28 +679,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -708,233 +708,239 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B37" s="7">
         <v>2014</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B48" s="7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B39" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B50" r:id="rId3" xr:uid="{0EAF8239-1601-435F-A7F3-DCBE0357401E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -944,15 +950,15 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="1" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -972,7 +978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -992,7 +998,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
@@ -1044,7 +1050,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -1116,7 +1122,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -1188,8 +1194,8 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1212,33 +1218,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <f>24*365</f>
         <v>8760</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3412.14</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.91400000000000003</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1253,18 +1261,18 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9">
         <v>2017</v>
@@ -1369,7 +1377,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1518,7 @@
         <v>1.3760295531402741E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1651,7 +1659,7 @@
         <v>2.7826375407947768E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>8.1644420152989595E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1933,149 +1941,150 @@
         <v>8.1644420152989595E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B6" s="11">
+        <f>B3*0.85</f>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:R6" si="20">$B6</f>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="D6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="E6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="F6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="G6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="H6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="I6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="J6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="K6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="L6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="M6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="N6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="O6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="P6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="Q6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="R6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="S6">
         <f t="shared" ref="S6:AI6" si="21">$B6</f>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="T6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="U6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="V6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="W6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="X6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="Y6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="Z6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AA6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AB6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AC6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AD6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AE6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AF6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AG6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AH6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AI6">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+        <v>2.3652419096755601E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B7" s="11">
         <f>B2</f>
@@ -2214,9 +2223,9 @@
         <v>1.3760295531402741E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B8" s="11">
         <f>B3</f>
@@ -2367,18 +2376,18 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AI8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B1" s="9">
         <v>2017</v>
@@ -2483,7 +2492,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2624,7 +2633,7 @@
         <v>2.0640443297104109E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2765,7 +2774,7 @@
         <v>1.307839644173545E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>4.0822210076494796E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3047,149 +3056,150 @@
         <v>4.0822210076494796E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B6" s="11">
+        <f>B3*0.95</f>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:AI6" si="1">$B6</f>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="R6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="W6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="Y6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="Z6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AB6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AC6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AD6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AE6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AF6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AG6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AI6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+        <v>1.2424476619648677E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B7" s="11">
         <f>B2</f>
@@ -3328,9 +3338,9 @@
         <v>2.0640443297104109E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B8" s="11">
         <f>B3</f>

</xml_diff>